<commit_message>
Enhance invoice Excel generation and UI components
- Added branchName to the Excel generation payload, allowing for better identification of the branch in the output.
- Updated the logic for determining the region internal code based on the branch name, improving accuracy in generated documents.
- Refactored the Invoice and Invoices components to enhance user experience, including improved error handling and visibility of task statuses.
- Adjusted the layout and styling of the Invoices component for better readability and interaction.
</commit_message>
<xml_diff>
--- a/backend/templates/CommodityEk_New2.xlsx
+++ b/backend/templates/CommodityEk_New2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Prodeklarant\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8731CA-96CB-4026-879B-A0E0F65C1DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588EFF1D-8266-46C4-A0F0-C101F87634ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5903,7 +5903,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6041,15 +6041,6 @@
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6357,10 +6348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="64" defaultRowHeight="15.75"/>
@@ -6523,276 +6514,6 @@
       <c r="V3" s="37"/>
       <c r="W3" s="37"/>
       <c r="X3" s="38"/>
-    </row>
-    <row r="4" spans="1:24" s="48" customFormat="1">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-    </row>
-    <row r="5" spans="1:24" s="48" customFormat="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47"/>
-    </row>
-    <row r="6" spans="1:24" s="48" customFormat="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
-    </row>
-    <row r="7" spans="1:24" s="48" customFormat="1">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47"/>
-    </row>
-    <row r="8" spans="1:24" s="48" customFormat="1">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="47"/>
-    </row>
-    <row r="9" spans="1:24" s="48" customFormat="1">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="47"/>
-    </row>
-    <row r="10" spans="1:24" s="48" customFormat="1">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47"/>
-    </row>
-    <row r="11" spans="1:24" s="48" customFormat="1">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47"/>
-    </row>
-    <row r="12" spans="1:24" s="48" customFormat="1">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:24" s="48" customFormat="1">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
-    </row>
-    <row r="14" spans="1:24" s="48" customFormat="1">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47"/>
-    </row>
-    <row r="15" spans="1:24" s="48" customFormat="1">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="47"/>
-    </row>
-    <row r="16" spans="1:24" s="48" customFormat="1">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="47"/>
-    </row>
-    <row r="17" spans="1:8" s="48" customFormat="1">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="47"/>
-    </row>
-    <row r="18" spans="1:8" s="48" customFormat="1">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="47"/>
-    </row>
-    <row r="19" spans="1:8" s="48" customFormat="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47"/>
-    </row>
-    <row r="20" spans="1:8" s="48" customFormat="1">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="47"/>
-    </row>
-    <row r="21" spans="1:8" s="48" customFormat="1">
-      <c r="A21" s="46"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="47"/>
-    </row>
-    <row r="22" spans="1:8" s="48" customFormat="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="47"/>
-    </row>
-    <row r="23" spans="1:8" s="48" customFormat="1">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="47"/>
-    </row>
-    <row r="24" spans="1:8" s="48" customFormat="1">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="47"/>
-    </row>
-    <row r="25" spans="1:8" s="48" customFormat="1">
-      <c r="A25" s="46"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="47"/>
-    </row>
-    <row r="26" spans="1:8" s="48" customFormat="1">
-      <c r="A26" s="46"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="47"/>
-    </row>
-    <row r="27" spans="1:8" s="48" customFormat="1">
-      <c r="A27" s="46"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="47"/>
-    </row>
-    <row r="28" spans="1:8" s="48" customFormat="1">
-      <c r="A28" s="46"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="47"/>
-    </row>
-    <row r="29" spans="1:8" s="48" customFormat="1">
-      <c r="A29" s="46"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="47"/>
-    </row>
-    <row r="30" spans="1:8" s="48" customFormat="1">
-      <c r="A30" s="46"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>